<commit_message>
267 : fix : 2.2 section
</commit_message>
<xml_diff>
--- a/text/pics/text_2_decompsurf/data.xlsx
+++ b/text/pics/text_2_decompsurf/data.xlsx
@@ -186,9 +186,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="3.6305652669146232E-2"/>
-          <c:y val="2.5731813340788764E-2"/>
-          <c:w val="0.95335565665125088"/>
-          <c:h val="0.81423025740937982"/>
+          <c:y val="2.5731813340788768E-2"/>
+          <c:w val="0.95335565665125099"/>
+          <c:h val="0.81423025740937993"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1094,11 +1094,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="125565568"/>
-        <c:axId val="125391232"/>
+        <c:axId val="144019840"/>
+        <c:axId val="144021376"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="125565568"/>
+        <c:axId val="144019840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1116,7 +1116,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="125391232"/>
+        <c:crossAx val="144021376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1124,7 +1124,7 @@
         <c:tickMarkSkip val="5"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="125391232"/>
+        <c:axId val="144021376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="50"/>
@@ -1144,7 +1144,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="125565568"/>
+        <c:crossAx val="144019840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="5"/>
@@ -1158,7 +1158,7 @@
           <c:yMode val="edge"/>
           <c:x val="1.743213159079671E-2"/>
           <c:y val="0.90984065481243781"/>
-          <c:w val="0.9713606156399861"/>
+          <c:w val="0.97136061563998621"/>
           <c:h val="7.0298316907787969E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -1177,7 +1177,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1195,8 +1195,8 @@
           <c:yMode val="edge"/>
           <c:x val="3.6305652669146232E-2"/>
           <c:y val="2.5731813340788771E-2"/>
-          <c:w val="0.9533556566512511"/>
-          <c:h val="0.81423025740938004"/>
+          <c:w val="0.95335565665125122"/>
+          <c:h val="0.81423025740938015"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -2102,11 +2102,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="125433728"/>
-        <c:axId val="125435264"/>
+        <c:axId val="144121216"/>
+        <c:axId val="144135296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="125433728"/>
+        <c:axId val="144121216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2124,7 +2124,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="125435264"/>
+        <c:crossAx val="144135296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2132,7 +2132,7 @@
         <c:tickMarkSkip val="5"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="125435264"/>
+        <c:axId val="144135296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -2151,7 +2151,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="125433728"/>
+        <c:crossAx val="144121216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="5"/>
@@ -2165,7 +2165,7 @@
           <c:yMode val="edge"/>
           <c:x val="1.743213159079671E-2"/>
           <c:y val="0.90984065481243781"/>
-          <c:w val="0.97136061563998632"/>
+          <c:w val="0.97136061563998644"/>
           <c:h val="7.0298316907787969E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -2184,7 +2184,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2202,8 +2202,8 @@
           <c:yMode val="edge"/>
           <c:x val="3.6305652669146232E-2"/>
           <c:y val="2.5731813340788771E-2"/>
-          <c:w val="0.95335565665125133"/>
-          <c:h val="0.81423025740938026"/>
+          <c:w val="0.95335565665125144"/>
+          <c:h val="0.81423025740938049"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -3082,11 +3082,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="156607616"/>
-        <c:axId val="156609152"/>
+        <c:axId val="144161408"/>
+        <c:axId val="144175488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="156607616"/>
+        <c:axId val="144161408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3104,7 +3104,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="156609152"/>
+        <c:crossAx val="144175488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3112,7 +3112,7 @@
         <c:tickMarkSkip val="5"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="156609152"/>
+        <c:axId val="144175488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="500"/>
@@ -3131,7 +3131,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="156607616"/>
+        <c:crossAx val="144161408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="50"/>
@@ -3145,7 +3145,7 @@
           <c:yMode val="edge"/>
           <c:x val="1.743213159079671E-2"/>
           <c:y val="0.90984065481243781"/>
-          <c:w val="0.97136061563998655"/>
+          <c:w val="0.97136061563998666"/>
           <c:h val="7.0298316907787969E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -3164,7 +3164,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3182,8 +3182,8 @@
           <c:yMode val="edge"/>
           <c:x val="3.6305652669146232E-2"/>
           <c:y val="2.5731813340788771E-2"/>
-          <c:w val="0.9533556566512511"/>
-          <c:h val="0.81423025740938004"/>
+          <c:w val="0.95335565665125122"/>
+          <c:h val="0.81423025740938015"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -4089,11 +4089,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="157700480"/>
-        <c:axId val="157702016"/>
+        <c:axId val="143558528"/>
+        <c:axId val="143560064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="157700480"/>
+        <c:axId val="143558528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4111,7 +4111,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="157702016"/>
+        <c:crossAx val="143560064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4119,7 +4119,7 @@
         <c:tickMarkSkip val="5"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="157702016"/>
+        <c:axId val="143560064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="50"/>
@@ -4138,7 +4138,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="157700480"/>
+        <c:crossAx val="143558528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="5"/>
@@ -4152,7 +4152,7 @@
           <c:yMode val="edge"/>
           <c:x val="1.743213159079671E-2"/>
           <c:y val="0.90984065481243781"/>
-          <c:w val="0.97136061563998632"/>
+          <c:w val="0.97136061563998644"/>
           <c:h val="7.0298316907787969E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -4171,7 +4171,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4189,8 +4189,8 @@
           <c:yMode val="edge"/>
           <c:x val="3.6305652669146232E-2"/>
           <c:y val="2.5731813340788771E-2"/>
-          <c:w val="0.95335565665125133"/>
-          <c:h val="0.81423025740938026"/>
+          <c:w val="0.95335565665125144"/>
+          <c:h val="0.81423025740938049"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -5096,11 +5096,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="157744512"/>
-        <c:axId val="157566080"/>
+        <c:axId val="145966208"/>
+        <c:axId val="145967744"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="157744512"/>
+        <c:axId val="145966208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5118,7 +5118,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="157566080"/>
+        <c:crossAx val="145967744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5126,7 +5126,7 @@
         <c:tickMarkSkip val="5"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="157566080"/>
+        <c:axId val="145967744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -5145,7 +5145,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="157744512"/>
+        <c:crossAx val="145966208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="5"/>
@@ -5159,7 +5159,7 @@
           <c:yMode val="edge"/>
           <c:x val="1.743213159079671E-2"/>
           <c:y val="0.90984065481243781"/>
-          <c:w val="0.97136061563998655"/>
+          <c:w val="0.97136061563998666"/>
           <c:h val="7.0298316907787969E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -5178,7 +5178,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5196,8 +5196,8 @@
           <c:yMode val="edge"/>
           <c:x val="3.6305652669146232E-2"/>
           <c:y val="2.5731813340788771E-2"/>
-          <c:w val="0.95335565665125155"/>
-          <c:h val="0.81423025740938071"/>
+          <c:w val="0.95335565665125166"/>
+          <c:h val="0.81423025740938082"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -6034,11 +6034,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="157608576"/>
-        <c:axId val="157618560"/>
+        <c:axId val="145998208"/>
+        <c:axId val="145999744"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="157608576"/>
+        <c:axId val="145998208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6056,7 +6056,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="157618560"/>
+        <c:crossAx val="145999744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6064,7 +6064,7 @@
         <c:tickMarkSkip val="5"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="157618560"/>
+        <c:axId val="145999744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10000"/>
@@ -6083,7 +6083,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="157608576"/>
+        <c:crossAx val="145998208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="1000"/>
@@ -6097,7 +6097,7 @@
           <c:yMode val="edge"/>
           <c:x val="1.743213159079671E-2"/>
           <c:y val="0.90984065481243781"/>
-          <c:w val="0.97136061563998677"/>
+          <c:w val="0.97136061563998688"/>
           <c:h val="7.0298316907787969E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -6116,7 +6116,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6594,8 +6594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:T99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="R106" sqref="R106"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H91" sqref="H91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>